<commit_message>
new things.... don't remember everything
</commit_message>
<xml_diff>
--- a/Cloud Solutions/student tracking/MCS student tracking 2223.xlsx
+++ b/Cloud Solutions/student tracking/MCS student tracking 2223.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\INTHECLOUD\Cloud Solutions\student tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4398F459-9E08-467D-AF94-434242A07BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9942A3D3-9C0C-40BA-96F1-901C3B07C2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="77">
   <si>
     <t>General Information</t>
   </si>
@@ -249,13 +249,19 @@
     <t>Time: voor het gehele project</t>
   </si>
   <si>
-    <t>Achievable: een script maken voor het inistializen van de website in azure</t>
-  </si>
-  <si>
     <t>Realistic: een begin gemaakt aan een script</t>
   </si>
   <si>
     <t>Time: eind van de week</t>
+  </si>
+  <si>
+    <t>Achievable: een script maken voor het inistialiseren van de website in azure</t>
+  </si>
+  <si>
+    <t>maak het scherper, beschrijf duidelijker wat je er van wilt zodat je opdrachtgever en jijzelf weet wat er wordt verwacht</t>
+  </si>
+  <si>
+    <t>dit is vooral belangrijk zodat er geen extra opdrachten/taken te voorschein komen en er geen misverstanden onstaan</t>
   </si>
 </sst>
 </file>
@@ -371,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -446,6 +452,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -913,7 +925,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -926,8 +938,8 @@
   </sheetPr>
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1558,6 +1570,9 @@
       <c r="B19" s="24" t="s">
         <v>66</v>
       </c>
+      <c r="D19" s="31" t="s">
+        <v>75</v>
+      </c>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
     </row>
@@ -1568,6 +1583,9 @@
       <c r="B20" s="24" t="s">
         <v>67</v>
       </c>
+      <c r="D20" s="32" t="s">
+        <v>76</v>
+      </c>
       <c r="E20" s="29"/>
       <c r="F20" s="29"/>
     </row>
@@ -1576,7 +1594,7 @@
         <v>69</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E21" s="29"/>
       <c r="F21" s="29"/>
@@ -1586,7 +1604,7 @@
         <v>70</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E22" s="29"/>
       <c r="F22" s="29"/>
@@ -1596,7 +1614,7 @@
         <v>71</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E23" s="29"/>
       <c r="F23" s="29"/>
@@ -2323,6 +2341,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EEE9BD865E9E914FBF0D3327E80C9312" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="2ae1e7e75a716937c3cc29f85ff05926">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f1a9ec08-63c2-477e-9fab-18773d342144" xmlns:ns3="3e072789-93b2-444e-af01-5faae066872a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eb35f4bddbfcf622dda5e81e85b23ac7" ns2:_="" ns3:_="">
     <xsd:import namespace="f1a9ec08-63c2-477e-9fab-18773d342144"/>
@@ -2547,15 +2574,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2568,6 +2586,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DDD8A64-C817-49D9-BDD2-DA29189A9B79}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D9E6AD2-0790-4ADF-AE6B-C3608D65A08D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2582,14 +2608,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DDD8A64-C817-49D9-BDD2-DA29189A9B79}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
added picturepoint just for safekeeping
</commit_message>
<xml_diff>
--- a/Cloud Solutions/student tracking/MCS student tracking 2223.xlsx
+++ b/Cloud Solutions/student tracking/MCS student tracking 2223.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\INTHECLOUD\Cloud Solutions\student tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9942A3D3-9C0C-40BA-96F1-901C3B07C2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5433B1-FFDB-42FF-8E68-41CE7AA2B4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="feedback approval form" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="82">
   <si>
     <t>General Information</t>
   </si>
@@ -262,6 +263,21 @@
   </si>
   <si>
     <t>dit is vooral belangrijk zodat er geen extra opdrachten/taken te voorschein komen en er geen misverstanden onstaan</t>
+  </si>
+  <si>
+    <t>Specific: Ik ben van plan voor het eind van deze sprint meerdere tests maken binnen de yml en dat dan over de code die we nu hebben te laten gaan</t>
+  </si>
+  <si>
+    <t>Measurable: dit wordt dan measurable door de tests te zien in de pipeline</t>
+  </si>
+  <si>
+    <t>Achievable: dit is haalbaar aangezien we genoeg code hebben, en er genoeg documentatie online staat</t>
+  </si>
+  <si>
+    <t>Realistic: dit is realistisch omdat het niet overdreven ingewikkelde code is en daarbij mogelijkheid is om het in de pipeline te laten testen</t>
+  </si>
+  <si>
+    <t>Time: ik heb hier de tijd van de sprint van 3 weken genomen</t>
   </si>
 </sst>
 </file>
@@ -448,7 +464,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -938,8 +954,8 @@
   </sheetPr>
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1857,51 +1873,41 @@
     </row>
     <row r="47" spans="1:6" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B47" s="24" t="s">
-        <v>32</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="B47" s="24"/>
       <c r="E47" s="29"/>
       <c r="F47" s="29"/>
     </row>
     <row r="48" spans="1:6" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B48" s="24" t="s">
-        <v>33</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B48" s="24"/>
       <c r="E48" s="29"/>
       <c r="F48" s="29"/>
     </row>
     <row r="49" spans="1:6" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B49" s="24" t="s">
-        <v>36</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B49" s="24"/>
       <c r="E49" s="29"/>
       <c r="F49" s="29"/>
     </row>
     <row r="50" spans="1:6" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B50" s="24" t="s">
-        <v>35</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="B50" s="24"/>
       <c r="E50" s="29"/>
       <c r="F50" s="29"/>
     </row>
     <row r="51" spans="1:6" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B51" s="24" t="s">
-        <v>34</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="B51" s="24"/>
       <c r="E51" s="29"/>
       <c r="F51" s="29"/>
     </row>
@@ -2341,15 +2347,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EEE9BD865E9E914FBF0D3327E80C9312" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="2ae1e7e75a716937c3cc29f85ff05926">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f1a9ec08-63c2-477e-9fab-18773d342144" xmlns:ns3="3e072789-93b2-444e-af01-5faae066872a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eb35f4bddbfcf622dda5e81e85b23ac7" ns2:_="" ns3:_="">
     <xsd:import namespace="f1a9ec08-63c2-477e-9fab-18773d342144"/>
@@ -2574,6 +2571,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2586,14 +2592,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DDD8A64-C817-49D9-BDD2-DA29189A9B79}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D9E6AD2-0790-4ADF-AE6B-C3608D65A08D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2608,6 +2606,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DDD8A64-C817-49D9-BDD2-DA29189A9B79}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>